<commit_message>
Add and update semester notes and control files
Added new control files for ELMO, ELRE, IELE, and PELE, as well as updated numeric notes spreadsheets for each section. Also added a new IELE_PASS_NOTES file and renamed the calendar file for the 2025-2026 school year.
</commit_message>
<xml_diff>
--- a/00-Administratif/01-ETIQUETTES + NOMBRE  NOTES SEMESTRIELLES/ELMO/ETIQUETTES NUMERIQUES/ELMO_NOTES.xlsx
+++ b/00-Administratif/01-ETIQUETTES + NOMBRE  NOTES SEMESTRIELLES/ELMO/ETIQUETTES NUMERIQUES/ELMO_NOTES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEXTES\EPSIC\ADMIN\ADMIN_DOMAINE_SANDRO\EXCEL_NOTES_DOMAINE_3\SHARE_POINT_ETIQUETTES_NUMERIQUES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB69031-EEEC-4C58-8C85-56EC140DAE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF42CE6A-6098-4416-A272-B7D14EADFA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24446EAE-FF7B-4720-8461-B68F93A38A30}"/>
   </bookViews>
@@ -1085,20 +1085,20 @@
     <t>Semestres</t>
   </si>
   <si>
-    <t>Moyenne de «CP» 4 ans</t>
+    <t>EIT.SWISS PQ ELMO</t>
   </si>
   <si>
-    <t>Moyenne d'«ECG» 4 ans</t>
+    <t>Moyenne d'«ECG» 3 ans</t>
   </si>
   <si>
-    <t>EIT.SWISS PQ ELMO</t>
+    <t>Moyenne de «CP» 3 ans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2119,13 +2119,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="15"/>
+    <col min="1" max="9" width="8.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45" customHeight="1">
+    <row r="1" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2141,12 +2141,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z2" s="15">
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.15" customHeight="1">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2160,12 +2160,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z4" s="15">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" customHeight="1">
+    <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
@@ -2181,12 +2181,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z6" s="15">
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>3</v>
       </c>
@@ -2208,12 +2208,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z8" s="15">
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" thickBot="1">
+    <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="13"/>
@@ -2274,7 +2274,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15" thickBot="1">
+    <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -2291,7 +2291,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2332,7 +2332,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="15" thickBot="1">
+    <row r="17" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="13"/>
@@ -2343,7 +2343,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="15" thickBot="1">
+    <row r="18" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -2360,7 +2360,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2401,7 +2401,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="15" thickBot="1">
+    <row r="22" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2412,7 +2412,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="23" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="1:26" ht="15" thickBot="1">
+    <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2441,7 +2441,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1">
+    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -2462,8 +2462,8 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15" thickTop="1"/>
-    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="26" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="18" t="s">
         <v>13</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="I27" s="18"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2503,7 +2503,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15" thickBot="1">
+    <row r="30" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -2514,7 +2514,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15" thickBot="1">
+    <row r="31" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -2531,7 +2531,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -2546,7 +2546,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -2557,7 +2557,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2568,7 +2568,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2585,7 +2585,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2596,7 +2596,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
@@ -2617,13 +2617,13 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickTop="1"/>
-    <row r="40" spans="1:9">
+    <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2727,13 +2727,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="15"/>
+    <col min="1" max="9" width="8.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45" customHeight="1">
+    <row r="1" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2749,12 +2749,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z2" s="15">
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.15" customHeight="1">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2768,12 +2768,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z4" s="15">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" customHeight="1">
+    <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
@@ -2789,12 +2789,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z6" s="15">
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>19</v>
       </c>
@@ -2816,12 +2816,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z8" s="15">
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" thickBot="1">
+    <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -2882,7 +2882,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15" thickBot="1">
+    <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -2899,7 +2899,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2914,7 +2914,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2929,7 +2929,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="13"/>
@@ -2940,7 +2940,7 @@
       <c r="H16" s="13"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="15" thickBot="1">
+    <row r="17" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="13"/>
@@ -2951,7 +2951,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="15" thickBot="1">
+    <row r="18" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -2968,7 +2968,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -2983,7 +2983,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2999,7 +2999,7 @@
       <c r="I20" s="2"/>
       <c r="O20" s="13"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -3010,7 +3010,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="15" thickBot="1">
+    <row r="22" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -3021,7 +3021,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="23" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="1:26" ht="15" thickBot="1">
+    <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3050,7 +3050,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1">
+    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3071,8 +3071,8 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15" thickTop="1"/>
-    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="26" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="18" t="s">
         <v>13</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="I27" s="18"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -3101,7 +3101,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -3112,7 +3112,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15" thickBot="1">
+    <row r="30" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3123,7 +3123,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15" thickBot="1">
+    <row r="31" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3140,7 +3140,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3153,7 +3153,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -3164,7 +3164,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3175,7 +3175,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3192,7 +3192,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3203,7 +3203,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
@@ -3224,13 +3224,13 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickTop="1"/>
-    <row r="40" spans="1:9">
+    <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -3360,13 +3360,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="15"/>
+    <col min="1" max="9" width="8.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45" customHeight="1">
+    <row r="1" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3382,12 +3382,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z2" s="15">
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.15" customHeight="1">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3401,12 +3401,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z4" s="15">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" customHeight="1">
+    <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
@@ -3422,12 +3422,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z6" s="15">
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
@@ -3449,12 +3449,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Z8" s="15">
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="13"/>
@@ -3504,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" thickBot="1">
+    <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="13"/>
@@ -3515,7 +3515,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15" thickBot="1">
+    <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -3532,7 +3532,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -3573,7 +3573,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="15" thickBot="1">
+    <row r="17" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="13"/>
@@ -3584,7 +3584,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="15" thickBot="1">
+    <row r="18" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -3601,7 +3601,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3612,7 +3612,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3623,7 +3623,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3634,7 +3634,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3645,7 +3645,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1">
+    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3657,7 +3657,7 @@
       <c r="I23" s="2"/>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="1:26" ht="15" thickBot="1">
+    <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3668,7 +3668,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1">
+    <row r="25" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3689,8 +3689,8 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15" thickTop="1"/>
-    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="26" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="18" t="s">
         <v>13</v>
       </c>
@@ -3704,7 +3704,7 @@
       <c r="I27" s="18"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -3730,7 +3730,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15" thickBot="1">
+    <row r="30" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3741,7 +3741,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15" thickBot="1">
+    <row r="31" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3758,7 +3758,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -3773,7 +3773,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -3784,7 +3784,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3795,7 +3795,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3812,7 +3812,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3823,7 +3823,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
@@ -3844,13 +3844,13 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickTop="1"/>
-    <row r="40" spans="1:9">
+    <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -3922,12 +3922,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.7109375" customWidth="1"/>
+    <col min="1" max="9" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" customHeight="1">
+    <row r="1" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3940,7 +3940,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="3" spans="1:22" s="5" customFormat="1" ht="25.15" customHeight="1">
+    <row r="3" spans="1:22" s="5" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3951,7 +3951,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="5" spans="1:22" ht="30" customHeight="1">
+    <row r="5" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
@@ -3964,7 +3964,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
@@ -3978,12 +3978,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" thickBot="1">
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="V8" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" thickBot="1">
+    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>3</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1">
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>5</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" thickBot="1">
+    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
@@ -4025,7 +4025,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="15" thickBot="1">
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>20</v>
       </c>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="15" thickBot="1">
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="15" thickBot="1">
+    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>24</v>
       </c>
@@ -4061,16 +4061,16 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="15" thickBot="1">
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="15.6" thickTop="1" thickBot="1">
+    <row r="16" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -4080,8 +4080,8 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="15" thickTop="1"/>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
         <v>13</v>
       </c>
@@ -4094,8 +4094,8 @@
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1"/>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>3</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>5</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
         <v>19</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>20</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>23</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
         <v>24</v>
       </c>
@@ -4161,14 +4161,14 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="27" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -4179,13 +4179,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickTop="1"/>
-    <row r="29" spans="1:9">
+    <row r="28" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -4252,15 +4252,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3874C8AB-05B1-4391-9816-BAA6BC768905}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -4284,17 +4284,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="28ecda99-baeb-4159-826c-8d3ebe501c98" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4303,9 +4292,9 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7262808F74C1A479C3BB44A303B6A0F" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="cab4a3c0111c554b2187f2cf1b3f650e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1" xmlns:ns3="28ecda99-baeb-4159-826c-8d3ebe501c98" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e122d3143e7eb9975e5aea102f87885" ns2:_="" ns3:_="">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7262808F74C1A479C3BB44A303B6A0F" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="53ca5ba934d9ea82b208c5ebaa87ee73">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1" xmlns:ns3="28ecda99-baeb-4159-826c-8d3ebe501c98" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="61005504990099e8d9d64d1794496304" ns2:_="" ns3:_="">
     <xsd:import namespace="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1"/>
     <xsd:import namespace="28ecda99-baeb-4159-826c-8d3ebe501c98"/>
     <xsd:element name="properties">
@@ -4327,6 +4316,7 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4387,6 +4377,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="22" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -4532,14 +4527,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="28ecda99-baeb-4159-826c-8d3ebe501c98" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CD9735-D523-4BAA-9E32-583B1ED165D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09B4E12-C5B5-423D-A5B0-596A57297A8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09B4E12-C5B5-423D-A5B0-596A57297A8E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AFB0D1E-F2E8-4EDD-8681-BD64330BFF8E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BA45EA5-E040-4330-83CE-A943DAED4818}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CD9735-D523-4BAA-9E32-583B1ED165D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81e70d26-bf48-4cf6-8ac1-a02ba5208bf1"/>
+    <ds:schemaRef ds:uri="28ecda99-baeb-4159-826c-8d3ebe501c98"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>